<commit_message>
Test Manifest         + Two Manifests with the same number         + No TPA, No TTT         + Not Existing Customer         + Not Existing Supplier         + Manifest with wrong Manifest Code
</commit_message>
<xml_diff>
--- a/src/test/resources/excelTests/manifestUploadGoodForecast.xlsx
+++ b/src/test/resources/excelTests/manifestUploadGoodForecast.xlsx
@@ -1242,6 +1242,7 @@
     <xf numFmtId="21" fontId="0" fillId="13" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="6" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="6" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="13" borderId="18" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="11" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1335,7 +1336,6 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="13" borderId="18" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Гиперссылка" xfId="1" builtinId="8"/>
@@ -1747,7 +1747,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="R18" sqref="R18"/>
+      <selection pane="bottomLeft" activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1772,42 +1772,42 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="77" t="s">
+      <c r="A1" s="78" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="78"/>
-      <c r="C1" s="78"/>
-      <c r="D1" s="79"/>
-      <c r="E1" s="89" t="s">
+      <c r="B1" s="79"/>
+      <c r="C1" s="79"/>
+      <c r="D1" s="80"/>
+      <c r="E1" s="90" t="s">
         <v>26</v>
       </c>
-      <c r="F1" s="89"/>
-      <c r="G1" s="89"/>
-      <c r="H1" s="90"/>
-      <c r="I1" s="91" t="s">
+      <c r="F1" s="90"/>
+      <c r="G1" s="90"/>
+      <c r="H1" s="91"/>
+      <c r="I1" s="92" t="s">
         <v>25</v>
       </c>
-      <c r="J1" s="92"/>
-      <c r="K1" s="92"/>
-      <c r="L1" s="92"/>
-      <c r="M1" s="86" t="s">
+      <c r="J1" s="93"/>
+      <c r="K1" s="93"/>
+      <c r="L1" s="93"/>
+      <c r="M1" s="87" t="s">
         <v>24</v>
       </c>
-      <c r="N1" s="87"/>
-      <c r="O1" s="87"/>
-      <c r="P1" s="88"/>
-      <c r="Q1" s="80" t="s">
+      <c r="N1" s="88"/>
+      <c r="O1" s="88"/>
+      <c r="P1" s="89"/>
+      <c r="Q1" s="81" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="81"/>
-      <c r="S1" s="82"/>
-      <c r="T1" s="83" t="s">
+      <c r="R1" s="82"/>
+      <c r="S1" s="83"/>
+      <c r="T1" s="84" t="s">
         <v>19</v>
       </c>
-      <c r="U1" s="84"/>
-      <c r="V1" s="84"/>
-      <c r="W1" s="84"/>
-      <c r="X1" s="85"/>
+      <c r="U1" s="85"/>
+      <c r="V1" s="85"/>
+      <c r="W1" s="85"/>
+      <c r="X1" s="86"/>
       <c r="Y1" s="2"/>
       <c r="Z1" s="2"/>
     </row>
@@ -1892,7 +1892,7 @@
         <v>39</v>
       </c>
       <c r="B3" s="52" t="n">
-        <v>43902.0</v>
+        <v>43904.0</v>
       </c>
       <c r="C3" s="63" t="n">
         <v>0.4375</v>
@@ -1904,7 +1904,7 @@
         <v>114</v>
       </c>
       <c r="F3" s="43" t="n">
-        <v>43903.0</v>
+        <v>43905.0</v>
       </c>
       <c r="G3" s="45" t="n">
         <v>0.6458333333333334</v>
@@ -1920,7 +1920,7 @@
         <v>113</v>
       </c>
       <c r="N3" s="49" t="n">
-        <v>43905.0</v>
+        <v>43907.0</v>
       </c>
       <c r="O3" s="54" t="n">
         <v>0.4583333333333333</v>
@@ -1932,7 +1932,7 @@
         <v>138</v>
       </c>
       <c r="R3" s="50" t="n">
-        <v>43918.0</v>
+        <v>43920.0</v>
       </c>
       <c r="S3" s="74" t="n">
         <v>0.4166666666666667</v>
@@ -1961,7 +1961,7 @@
         <v>41</v>
       </c>
       <c r="B4" s="42" t="n">
-        <v>43901.0</v>
+        <v>43903.0</v>
       </c>
       <c r="C4" s="61" t="n">
         <v>0.4791666666666667</v>
@@ -1973,7 +1973,7 @@
         <v>115</v>
       </c>
       <c r="F4" s="44" t="n">
-        <v>43902.0</v>
+        <v>43903.0</v>
       </c>
       <c r="G4" s="45" t="n">
         <v>0.6875</v>
@@ -1985,7 +1985,7 @@
         <v>116</v>
       </c>
       <c r="J4" s="47" t="n">
-        <v>43904.0</v>
+        <v>43906.0</v>
       </c>
       <c r="K4" s="56" t="n">
         <v>0.6944444444444444</v>
@@ -1997,7 +1997,7 @@
         <v>113</v>
       </c>
       <c r="N4" s="46" t="n">
-        <v>43906.0</v>
+        <v>43908.0</v>
       </c>
       <c r="O4" s="53" t="n">
         <v>0.7083333333333334</v>
@@ -2009,9 +2009,9 @@
         <v>139</v>
       </c>
       <c r="R4" s="51" t="n">
-        <v>43910.0</v>
+        <v>43912.0</v>
       </c>
-      <c r="S4" s="108" t="n">
+      <c r="S4" s="77" t="n">
         <v>0.5</v>
       </c>
       <c r="T4" s="38" t="s">
@@ -2035,7 +2035,7 @@
         <v>89</v>
       </c>
       <c r="B5" s="42" t="n">
-        <v>43897.0</v>
+        <v>43899.0</v>
       </c>
       <c r="C5" s="61" t="n">
         <v>0.3541666666666667</v>
@@ -2047,7 +2047,7 @@
         <v>117</v>
       </c>
       <c r="F5" s="43" t="n">
-        <v>43900.0</v>
+        <v>43902.0</v>
       </c>
       <c r="G5" s="45" t="n">
         <v>0.4375</v>
@@ -2059,7 +2059,7 @@
         <v>116</v>
       </c>
       <c r="J5" s="47" t="n">
-        <v>43903.0</v>
+        <v>43905.0</v>
       </c>
       <c r="K5" s="56" t="n">
         <v>0.5798611111111112</v>
@@ -2075,9 +2075,9 @@
         <v>140</v>
       </c>
       <c r="R5" s="51" t="n">
-        <v>43904.0</v>
+        <v>43906.0</v>
       </c>
-      <c r="S5" s="108" t="n">
+      <c r="S5" s="77" t="n">
         <v>0.7083333333333334</v>
       </c>
       <c r="T5" s="38" t="s">
@@ -2257,24 +2257,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="93" t="s">
+      <c r="A1" s="94" t="s">
         <v>28</v>
       </c>
-      <c r="B1" s="93" t="s">
+      <c r="B1" s="94" t="s">
         <v>32</v>
       </c>
-      <c r="C1" s="93" t="s">
+      <c r="C1" s="94" t="s">
         <v>29</v>
       </c>
-      <c r="D1" s="93" t="s">
+      <c r="D1" s="94" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="94"/>
-      <c r="B2" s="94"/>
-      <c r="C2" s="94"/>
-      <c r="D2" s="94"/>
+      <c r="A2" s="95"/>
+      <c r="B2" s="95"/>
+      <c r="C2" s="95"/>
+      <c r="D2" s="95"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
@@ -2381,44 +2381,44 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="97" t="s">
+      <c r="A1" s="98" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="95" t="s">
+      <c r="B1" s="96" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="95" t="s">
+      <c r="C1" s="96" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="95" t="s">
+      <c r="D1" s="96" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="95" t="s">
+      <c r="E1" s="96" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="95" t="s">
+      <c r="F1" s="96" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="95" t="s">
+      <c r="G1" s="96" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="95" t="s">
+      <c r="H1" s="96" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="95" t="s">
+      <c r="I1" s="96" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="98"/>
-      <c r="B2" s="96"/>
-      <c r="C2" s="96"/>
-      <c r="D2" s="96"/>
-      <c r="E2" s="96"/>
-      <c r="F2" s="96"/>
-      <c r="G2" s="96"/>
-      <c r="H2" s="96"/>
-      <c r="I2" s="96"/>
+      <c r="A2" s="99"/>
+      <c r="B2" s="97"/>
+      <c r="C2" s="97"/>
+      <c r="D2" s="97"/>
+      <c r="E2" s="97"/>
+      <c r="F2" s="97"/>
+      <c r="G2" s="97"/>
+      <c r="H2" s="97"/>
+      <c r="I2" s="97"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
@@ -16262,48 +16262,48 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" s="103" t="s">
+      <c r="A1" s="104" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="99" t="s">
+      <c r="B1" s="100" t="s">
         <v>8</v>
       </c>
-      <c r="C1" s="99" t="s">
+      <c r="C1" s="100" t="s">
         <v>9</v>
       </c>
-      <c r="D1" s="101" t="s">
+      <c r="D1" s="102" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="101" t="s">
+      <c r="E1" s="102" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="99" t="s">
+      <c r="F1" s="100" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="99" t="s">
+      <c r="G1" s="100" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="99" t="s">
+      <c r="H1" s="100" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="101" t="s">
+      <c r="I1" s="102" t="s">
         <v>36</v>
       </c>
-      <c r="J1" s="99" t="s">
+      <c r="J1" s="100" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="104"/>
-      <c r="B2" s="100"/>
-      <c r="C2" s="100"/>
-      <c r="D2" s="105"/>
-      <c r="E2" s="105"/>
-      <c r="F2" s="100"/>
-      <c r="G2" s="100"/>
-      <c r="H2" s="100"/>
-      <c r="I2" s="102"/>
-      <c r="J2" s="100"/>
+      <c r="A2" s="105"/>
+      <c r="B2" s="101"/>
+      <c r="C2" s="101"/>
+      <c r="D2" s="106"/>
+      <c r="E2" s="106"/>
+      <c r="F2" s="101"/>
+      <c r="G2" s="101"/>
+      <c r="H2" s="101"/>
+      <c r="I2" s="103"/>
+      <c r="J2" s="101"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
@@ -33059,36 +33059,36 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="106" t="s">
+      <c r="A1" s="107" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="106" t="s">
+      <c r="B1" s="107" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="106" t="s">
+      <c r="C1" s="107" t="s">
         <v>5</v>
       </c>
-      <c r="D1" s="106" t="s">
+      <c r="D1" s="107" t="s">
         <v>6</v>
       </c>
-      <c r="E1" s="106" t="s">
+      <c r="E1" s="107" t="s">
         <v>7</v>
       </c>
-      <c r="F1" s="106" t="s">
+      <c r="F1" s="107" t="s">
         <v>11</v>
       </c>
-      <c r="G1" s="106" t="s">
+      <c r="G1" s="107" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="107"/>
-      <c r="B2" s="107"/>
-      <c r="C2" s="107"/>
-      <c r="D2" s="107"/>
-      <c r="E2" s="107"/>
-      <c r="F2" s="107"/>
-      <c r="G2" s="107"/>
+      <c r="A2" s="108"/>
+      <c r="B2" s="108"/>
+      <c r="C2" s="108"/>
+      <c r="D2" s="108"/>
+      <c r="E2" s="108"/>
+      <c r="F2" s="108"/>
+      <c r="G2" s="108"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">

</xml_diff>

<commit_message>
If Customer or Supplier has status isActive=false set manifest status to false Tests passed
</commit_message>
<xml_diff>
--- a/src/test/resources/excelTests/manifestUploadGoodForecast.xlsx
+++ b/src/test/resources/excelTests/manifestUploadGoodForecast.xlsx
@@ -1892,7 +1892,7 @@
         <v>39</v>
       </c>
       <c r="B3" s="52" t="n">
-        <v>43904.0</v>
+        <v>43908.0</v>
       </c>
       <c r="C3" s="63" t="n">
         <v>0.4375</v>
@@ -1904,7 +1904,7 @@
         <v>114</v>
       </c>
       <c r="F3" s="43" t="n">
-        <v>43905.0</v>
+        <v>43909.0</v>
       </c>
       <c r="G3" s="45" t="n">
         <v>0.6458333333333334</v>
@@ -1920,7 +1920,7 @@
         <v>113</v>
       </c>
       <c r="N3" s="49" t="n">
-        <v>43907.0</v>
+        <v>43911.0</v>
       </c>
       <c r="O3" s="54" t="n">
         <v>0.4583333333333333</v>
@@ -1932,7 +1932,7 @@
         <v>138</v>
       </c>
       <c r="R3" s="50" t="n">
-        <v>43920.0</v>
+        <v>43924.0</v>
       </c>
       <c r="S3" s="74" t="n">
         <v>0.4166666666666667</v>
@@ -1961,7 +1961,7 @@
         <v>41</v>
       </c>
       <c r="B4" s="42" t="n">
-        <v>43903.0</v>
+        <v>43907.0</v>
       </c>
       <c r="C4" s="61" t="n">
         <v>0.4791666666666667</v>
@@ -1973,7 +1973,7 @@
         <v>115</v>
       </c>
       <c r="F4" s="44" t="n">
-        <v>43903.0</v>
+        <v>43907.0</v>
       </c>
       <c r="G4" s="45" t="n">
         <v>0.6875</v>
@@ -1985,10 +1985,10 @@
         <v>116</v>
       </c>
       <c r="J4" s="47" t="n">
-        <v>43906.0</v>
+        <v>43910.0</v>
       </c>
       <c r="K4" s="56" t="n">
-        <v>0.6944444444444444</v>
+        <v>0.5277777777777778</v>
       </c>
       <c r="L4" s="13" t="s">
         <v>107</v>
@@ -1997,7 +1997,7 @@
         <v>113</v>
       </c>
       <c r="N4" s="46" t="n">
-        <v>43908.0</v>
+        <v>43912.0</v>
       </c>
       <c r="O4" s="53" t="n">
         <v>0.7083333333333334</v>
@@ -2009,7 +2009,7 @@
         <v>139</v>
       </c>
       <c r="R4" s="51" t="n">
-        <v>43912.0</v>
+        <v>43916.0</v>
       </c>
       <c r="S4" s="77" t="n">
         <v>0.5</v>
@@ -2035,7 +2035,7 @@
         <v>89</v>
       </c>
       <c r="B5" s="42" t="n">
-        <v>43899.0</v>
+        <v>43903.0</v>
       </c>
       <c r="C5" s="61" t="n">
         <v>0.3541666666666667</v>
@@ -2047,7 +2047,7 @@
         <v>117</v>
       </c>
       <c r="F5" s="43" t="n">
-        <v>43902.0</v>
+        <v>43906.0</v>
       </c>
       <c r="G5" s="45" t="n">
         <v>0.4375</v>
@@ -2059,7 +2059,7 @@
         <v>116</v>
       </c>
       <c r="J5" s="47" t="n">
-        <v>43905.0</v>
+        <v>43909.0</v>
       </c>
       <c r="K5" s="56" t="n">
         <v>0.5798611111111112</v>
@@ -2075,7 +2075,7 @@
         <v>140</v>
       </c>
       <c r="R5" s="51" t="n">
-        <v>43906.0</v>
+        <v>43910.0</v>
       </c>
       <c r="S5" s="77" t="n">
         <v>0.7083333333333334</v>

</xml_diff>

<commit_message>
If Forecast has manifest which has references with agreements which cannot be found in DB this manifest will have status isActive=False
</commit_message>
<xml_diff>
--- a/src/test/resources/excelTests/manifestUploadGoodForecast.xlsx
+++ b/src/test/resources/excelTests/manifestUploadGoodForecast.xlsx
@@ -1892,7 +1892,7 @@
         <v>39</v>
       </c>
       <c r="B3" s="52" t="n">
-        <v>43908.0</v>
+        <v>43909.0</v>
       </c>
       <c r="C3" s="63" t="n">
         <v>0.4375</v>
@@ -1904,7 +1904,7 @@
         <v>114</v>
       </c>
       <c r="F3" s="43" t="n">
-        <v>43909.0</v>
+        <v>43910.0</v>
       </c>
       <c r="G3" s="45" t="n">
         <v>0.6458333333333334</v>
@@ -1920,7 +1920,7 @@
         <v>113</v>
       </c>
       <c r="N3" s="49" t="n">
-        <v>43911.0</v>
+        <v>43912.0</v>
       </c>
       <c r="O3" s="54" t="n">
         <v>0.4583333333333333</v>
@@ -1932,7 +1932,7 @@
         <v>138</v>
       </c>
       <c r="R3" s="50" t="n">
-        <v>43924.0</v>
+        <v>43925.0</v>
       </c>
       <c r="S3" s="74" t="n">
         <v>0.4166666666666667</v>
@@ -1961,7 +1961,7 @@
         <v>41</v>
       </c>
       <c r="B4" s="42" t="n">
-        <v>43907.0</v>
+        <v>43908.0</v>
       </c>
       <c r="C4" s="61" t="n">
         <v>0.4791666666666667</v>
@@ -1973,7 +1973,7 @@
         <v>115</v>
       </c>
       <c r="F4" s="44" t="n">
-        <v>43907.0</v>
+        <v>43908.0</v>
       </c>
       <c r="G4" s="45" t="n">
         <v>0.6875</v>
@@ -1985,7 +1985,7 @@
         <v>116</v>
       </c>
       <c r="J4" s="47" t="n">
-        <v>43910.0</v>
+        <v>43911.0</v>
       </c>
       <c r="K4" s="56" t="n">
         <v>0.5277777777777778</v>
@@ -1997,7 +1997,7 @@
         <v>113</v>
       </c>
       <c r="N4" s="46" t="n">
-        <v>43912.0</v>
+        <v>43913.0</v>
       </c>
       <c r="O4" s="53" t="n">
         <v>0.7083333333333334</v>
@@ -2009,7 +2009,7 @@
         <v>139</v>
       </c>
       <c r="R4" s="51" t="n">
-        <v>43916.0</v>
+        <v>43917.0</v>
       </c>
       <c r="S4" s="77" t="n">
         <v>0.5</v>
@@ -2035,7 +2035,7 @@
         <v>89</v>
       </c>
       <c r="B5" s="42" t="n">
-        <v>43903.0</v>
+        <v>43904.0</v>
       </c>
       <c r="C5" s="61" t="n">
         <v>0.3541666666666667</v>
@@ -2047,7 +2047,7 @@
         <v>117</v>
       </c>
       <c r="F5" s="43" t="n">
-        <v>43906.0</v>
+        <v>43907.0</v>
       </c>
       <c r="G5" s="45" t="n">
         <v>0.4375</v>
@@ -2059,7 +2059,7 @@
         <v>116</v>
       </c>
       <c r="J5" s="47" t="n">
-        <v>43909.0</v>
+        <v>43910.0</v>
       </c>
       <c r="K5" s="56" t="n">
         <v>0.5798611111111112</v>
@@ -2075,7 +2075,7 @@
         <v>140</v>
       </c>
       <c r="R5" s="51" t="n">
-        <v>43910.0</v>
+        <v>43911.0</v>
       </c>
       <c r="S5" s="77" t="n">
         <v>0.7083333333333334</v>

</xml_diff>

<commit_message>
If ManifestReference doesnt have dedicated TPA it will be changed to isActive=false therefore Manifest Also.
</commit_message>
<xml_diff>
--- a/src/test/resources/excelTests/manifestUploadGoodForecast.xlsx
+++ b/src/test/resources/excelTests/manifestUploadGoodForecast.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" codeName="ЭтаКнига" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="MANIFESTS" sheetId="4" r:id="rId1"/>
@@ -65,7 +65,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="145">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="142">
   <si>
     <t>ID</t>
   </si>
@@ -395,13 +395,7 @@
     <t>44444XXX</t>
   </si>
   <si>
-    <t>11111XXX-CO</t>
-  </si>
-  <si>
     <t>11111YYY</t>
-  </si>
-  <si>
-    <t>false</t>
   </si>
   <si>
     <t>true</t>
@@ -522,9 +516,6 @@
   </si>
   <si>
     <t>440000000</t>
-  </si>
-  <si>
-    <t>4400022222</t>
   </si>
   <si>
     <t>440001111</t>
@@ -1745,7 +1736,7 @@
   <sheetPr codeName="Лист1"/>
   <dimension ref="A1:Z5"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="H4" sqref="H4"/>
     </sheetView>
@@ -1892,47 +1883,47 @@
         <v>39</v>
       </c>
       <c r="B3" s="52" t="n">
-        <v>43909.0</v>
+        <v>43911.0</v>
       </c>
       <c r="C3" s="63" t="n">
         <v>0.4375</v>
       </c>
       <c r="D3" s="63" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="E3" s="58" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="F3" s="43" t="n">
-        <v>43910.0</v>
+        <v>43912.0</v>
       </c>
       <c r="G3" s="45" t="n">
         <v>0.6458333333333334</v>
       </c>
       <c r="H3" s="33" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="I3" s="10"/>
       <c r="J3" s="48"/>
       <c r="K3" s="55"/>
       <c r="L3" s="12"/>
       <c r="M3" s="14" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="N3" s="49" t="n">
-        <v>43912.0</v>
+        <v>43914.0</v>
       </c>
       <c r="O3" s="54" t="n">
         <v>0.4583333333333333</v>
       </c>
       <c r="P3" s="15" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="Q3" s="16" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="R3" s="50" t="n">
-        <v>43925.0</v>
+        <v>43927.0</v>
       </c>
       <c r="S3" s="74" t="n">
         <v>0.4166666666666667</v>
@@ -1961,55 +1952,55 @@
         <v>41</v>
       </c>
       <c r="B4" s="42" t="n">
-        <v>43908.0</v>
+        <v>43910.0</v>
       </c>
       <c r="C4" s="61" t="n">
         <v>0.4791666666666667</v>
       </c>
       <c r="D4" s="61" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="E4" s="59" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="F4" s="44" t="n">
-        <v>43908.0</v>
+        <v>43910.0</v>
       </c>
       <c r="G4" s="45" t="n">
         <v>0.6875</v>
       </c>
       <c r="H4" s="9" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="I4" s="11" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="J4" s="47" t="n">
-        <v>43911.0</v>
+        <v>43913.0</v>
       </c>
       <c r="K4" s="56" t="n">
         <v>0.5277777777777778</v>
       </c>
       <c r="L4" s="13" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="M4" s="14" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="N4" s="46" t="n">
-        <v>43913.0</v>
+        <v>43915.0</v>
       </c>
       <c r="O4" s="53" t="n">
         <v>0.7083333333333334</v>
       </c>
       <c r="P4" s="15" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="Q4" s="17" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="R4" s="51" t="n">
-        <v>43917.0</v>
+        <v>43919.0</v>
       </c>
       <c r="S4" s="77" t="n">
         <v>0.5</v>
@@ -2035,47 +2026,47 @@
         <v>89</v>
       </c>
       <c r="B5" s="42" t="n">
-        <v>43904.0</v>
+        <v>43906.0</v>
       </c>
       <c r="C5" s="61" t="n">
         <v>0.3541666666666667</v>
       </c>
       <c r="D5" s="61" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="E5" s="59" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="F5" s="43" t="n">
-        <v>43907.0</v>
+        <v>43909.0</v>
       </c>
       <c r="G5" s="45" t="n">
         <v>0.4375</v>
       </c>
       <c r="H5" s="9" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="I5" s="11" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="J5" s="47" t="n">
-        <v>43910.0</v>
+        <v>43912.0</v>
       </c>
       <c r="K5" s="56" t="n">
         <v>0.5798611111111112</v>
       </c>
       <c r="L5" s="13" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="M5" s="14"/>
       <c r="N5" s="46"/>
       <c r="O5" s="53"/>
       <c r="P5" s="15"/>
       <c r="Q5" s="17" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="R5" s="51" t="n">
-        <v>43911.0</v>
+        <v>43913.0</v>
       </c>
       <c r="S5" s="77" t="n">
         <v>0.7083333333333334</v>
@@ -2141,11 +2132,11 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D3:D3000">
-    <cfRule type="expression" dxfId="9" priority="3">
+    <cfRule type="expression" dxfId="9" priority="2">
+      <formula>NOT(AND(B3=INDEX($B$3:$B$3000,MATCH(D3,$D$3:$D$3000,0)),C3=INDEX($C$3:$C$3000,MATCH(D3,$D$3:$D$3000,0))))</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="8" priority="3">
       <formula>AND(NOT(ISBLANK($A3)),ISBLANK($D3))</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="8" priority="2">
-      <formula>NOT(AND(B3=INDEX($B$3:$B$3000,MATCH(D3,$D$3:$D$3000,0)),C3=INDEX($C$3:$C$3000,MATCH(D3,$D$3:$D$3000,0))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T3:T3382">
@@ -2240,11 +2231,11 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Лист2"/>
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I16" sqref="I16"/>
+      <selection pane="bottomLeft" activeCell="A4" sqref="A4:XFD4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2281,7 +2272,7 @@
         <v>96</v>
       </c>
       <c r="B3" s="75" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>99</v>
@@ -2290,7 +2281,7 @@
         <v>10</v>
       </c>
       <c r="E3" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -2298,33 +2289,16 @@
         <v>97</v>
       </c>
       <c r="B4" s="76" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="C4" s="7" t="s">
         <v>100</v>
       </c>
       <c r="D4" s="8">
-        <v>100</v>
+        <v>1000</v>
       </c>
       <c r="E4" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="6" t="s">
-        <v>97</v>
-      </c>
-      <c r="B5" s="76" t="s">
-        <v>144</v>
-      </c>
-      <c r="C5" s="7" t="s">
         <v>101</v>
-      </c>
-      <c r="D5" s="8">
-        <v>1000</v>
-      </c>
-      <c r="E5" t="s">
-        <v>103</v>
       </c>
     </row>
   </sheetData>
@@ -2352,7 +2326,7 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>A3:A5</xm:sqref>
+          <xm:sqref>A3:A4</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>
@@ -2527,7 +2501,7 @@
         <v>80</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="H6" s="1" t="s">
         <v>81</v>
@@ -16310,7 +16284,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="C3" s="1">
         <v>123123</v>
@@ -16342,7 +16316,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="C4" s="1">
         <v>500500</v>
@@ -16357,7 +16331,7 @@
         <v>53</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="H4" s="1" t="s">
         <v>54</v>
@@ -16374,7 +16348,7 @@
         <v>3</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="C5" s="1">
         <v>777222</v>
@@ -16406,7 +16380,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="C6" s="1">
         <v>194978</v>
@@ -33092,117 +33066,117 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>37</v>
       </c>
       <c r="C3" s="72" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="E3" s="73" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="F3" s="1" t="s">
         <v>45</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>37</v>
       </c>
       <c r="C4" s="72" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="E4" s="73" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="F4" s="1" t="s">
         <v>44</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="C5" s="72" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="E5" s="73" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="F5" s="1" t="s">
         <v>45</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>38</v>
       </c>
       <c r="C6" s="72" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="E6" s="73" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="F6" s="1" t="s">
         <v>43</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="E7" s="73" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="F7" s="1" t="s">
         <v>45</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Check the condition of similarity of the Supplier and Customer of Manifest with the Supplier and Customer of Reference in each ManifestReference entity.
</commit_message>
<xml_diff>
--- a/src/test/resources/excelTests/manifestUploadGoodForecast.xlsx
+++ b/src/test/resources/excelTests/manifestUploadGoodForecast.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" codeName="ЭтаКнига" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
   </bookViews>
   <sheets>
     <sheet name="MANIFESTS" sheetId="4" r:id="rId1"/>
@@ -1736,9 +1736,9 @@
   <sheetPr codeName="Лист1"/>
   <dimension ref="A1:Z5"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H4" sqref="H4"/>
+      <selection pane="bottomLeft" activeCell="O10" sqref="O10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1883,7 +1883,7 @@
         <v>39</v>
       </c>
       <c r="B3" s="52" t="n">
-        <v>43911.0</v>
+        <v>43919.0</v>
       </c>
       <c r="C3" s="63" t="n">
         <v>0.4375</v>
@@ -1895,7 +1895,7 @@
         <v>112</v>
       </c>
       <c r="F3" s="43" t="n">
-        <v>43912.0</v>
+        <v>43920.0</v>
       </c>
       <c r="G3" s="45" t="n">
         <v>0.6458333333333334</v>
@@ -1911,7 +1911,7 @@
         <v>111</v>
       </c>
       <c r="N3" s="49" t="n">
-        <v>43914.0</v>
+        <v>43922.0</v>
       </c>
       <c r="O3" s="54" t="n">
         <v>0.4583333333333333</v>
@@ -1920,10 +1920,10 @@
         <v>109</v>
       </c>
       <c r="Q3" s="16" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="R3" s="50" t="n">
-        <v>43927.0</v>
+        <v>43935.0</v>
       </c>
       <c r="S3" s="74" t="n">
         <v>0.4166666666666667</v>
@@ -1952,7 +1952,7 @@
         <v>41</v>
       </c>
       <c r="B4" s="42" t="n">
-        <v>43910.0</v>
+        <v>43918.0</v>
       </c>
       <c r="C4" s="61" t="n">
         <v>0.4791666666666667</v>
@@ -1964,7 +1964,7 @@
         <v>113</v>
       </c>
       <c r="F4" s="44" t="n">
-        <v>43910.0</v>
+        <v>43918.0</v>
       </c>
       <c r="G4" s="45" t="n">
         <v>0.6875</v>
@@ -1976,7 +1976,7 @@
         <v>114</v>
       </c>
       <c r="J4" s="47" t="n">
-        <v>43913.0</v>
+        <v>43921.0</v>
       </c>
       <c r="K4" s="56" t="n">
         <v>0.5277777777777778</v>
@@ -1988,7 +1988,7 @@
         <v>111</v>
       </c>
       <c r="N4" s="46" t="n">
-        <v>43915.0</v>
+        <v>43923.0</v>
       </c>
       <c r="O4" s="53" t="n">
         <v>0.7083333333333334</v>
@@ -1997,10 +1997,10 @@
         <v>110</v>
       </c>
       <c r="Q4" s="17" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="R4" s="51" t="n">
-        <v>43919.0</v>
+        <v>43927.0</v>
       </c>
       <c r="S4" s="77" t="n">
         <v>0.5</v>
@@ -2026,7 +2026,7 @@
         <v>89</v>
       </c>
       <c r="B5" s="42" t="n">
-        <v>43906.0</v>
+        <v>43914.0</v>
       </c>
       <c r="C5" s="61" t="n">
         <v>0.3541666666666667</v>
@@ -2038,7 +2038,7 @@
         <v>115</v>
       </c>
       <c r="F5" s="43" t="n">
-        <v>43909.0</v>
+        <v>43917.0</v>
       </c>
       <c r="G5" s="45" t="n">
         <v>0.4375</v>
@@ -2050,7 +2050,7 @@
         <v>114</v>
       </c>
       <c r="J5" s="47" t="n">
-        <v>43912.0</v>
+        <v>43920.0</v>
       </c>
       <c r="K5" s="56" t="n">
         <v>0.5798611111111112</v>
@@ -2066,7 +2066,7 @@
         <v>138</v>
       </c>
       <c r="R5" s="51" t="n">
-        <v>43913.0</v>
+        <v>43921.0</v>
       </c>
       <c r="S5" s="77" t="n">
         <v>0.7083333333333334</v>
@@ -2233,7 +2233,7 @@
   <sheetPr codeName="Лист2"/>
   <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4:XFD4"/>
     </sheetView>
@@ -16221,7 +16221,7 @@
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B8" sqref="B8"/>
+      <selection pane="bottomLeft" activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>